<commit_message>
Inclusión del campo destino en las ordenes de compra
</commit_message>
<xml_diff>
--- a/Ppgz/Ppgz.Web/App_Data/plantillaoc.xlsx
+++ b/Ppgz/Ppgz.Web/App_Data/plantillaoc.xlsx
@@ -33,9 +33,6 @@
     <t>DESCRIPCIÓN</t>
   </si>
   <si>
-    <t>ALMACÉN</t>
-  </si>
-  <si>
     <t>PRECIO</t>
   </si>
   <si>
@@ -52,6 +49,9 @@
   </si>
   <si>
     <t>CANT</t>
+  </si>
+  <si>
+    <t>DESTINO</t>
   </si>
 </sst>
 </file>
@@ -239,20 +239,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,6 +256,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -630,22 +630,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="24"/>
+    </row>
+    <row r="2" spans="1:5" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="19"/>
+      <c r="B2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
-    </row>
-    <row r="2" spans="1:5" ht="80.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
@@ -655,8 +655,8 @@
       <c r="C3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="21"/>
     </row>
     <row r="4" spans="1:5" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
@@ -667,7 +667,7 @@
     </row>
     <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="9"/>
@@ -676,7 +676,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="9"/>
@@ -698,13 +698,13 @@
         <v>3</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>